<commit_message>
updated fsc template file
</commit_message>
<xml_diff>
--- a/webdata/FSEUploadTemplate.xlsx
+++ b/webdata/FSEUploadTemplate.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/B0208058/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/B0216779/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CED47C29-F6CF-EF4C-84AE-27C24FB11E08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCDEC5A-F108-7548-8C36-DF763C2A4251}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="1960" windowWidth="26840" windowHeight="14640" xr2:uid="{519E6761-B49C-2748-B17C-EFA8A0774656}"/>
+    <workbookView xWindow="4300" yWindow="2760" windowWidth="27640" windowHeight="16940" xr2:uid="{F51F200A-1BBF-B74F-91B8-EDD9C0D1CB1B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Format" sheetId="1" r:id="rId1"/>
+    <sheet name="Sample Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,36 +26,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>FSE VL No</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+  <si>
+    <t>Retailer Number</t>
   </si>
   <si>
     <t>Retailer Name</t>
   </si>
   <si>
-    <t>Retailer VL No</t>
-  </si>
-  <si>
     <t>Retailer Address</t>
   </si>
   <si>
+    <t>Date Of Camp (dd/mm/yyyy)</t>
+  </si>
+  <si>
+    <t>Target Acquisition</t>
+  </si>
+  <si>
+    <t>Target recharge amount</t>
+  </si>
+  <si>
+    <t>Target sim Swap</t>
+  </si>
+  <si>
+    <t>Target recharge count</t>
+  </si>
+  <si>
     <t>Retailer Lat Long</t>
   </si>
   <si>
-    <t>Date of Camp (dd/mm/yyyy)</t>
-  </si>
-  <si>
-    <t>Target Acquisition</t>
-  </si>
-  <si>
-    <t>Target recharge count</t>
-  </si>
-  <si>
-    <t>Target recharge amount</t>
-  </si>
-  <si>
-    <t>Target sim Swap</t>
+    <t>FSE ID(Lapu no)</t>
+  </si>
+  <si>
+    <t>753011513</t>
+  </si>
+  <si>
+    <t>Test Retailer</t>
+  </si>
+  <si>
+    <t>Orleans</t>
+  </si>
+  <si>
+    <t>7.873054/80.771797</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>8.873054/82.771797</t>
+  </si>
+  <si>
+    <t>Srilanka</t>
+  </si>
+  <si>
+    <t>918377891507</t>
+  </si>
+  <si>
+    <t>31/01/2021</t>
+  </si>
+  <si>
+    <t>30/01/2021</t>
   </si>
 </sst>
 </file>
@@ -90,8 +127,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,60 +443,176 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6EEF00-F7D7-A54D-8800-D4BCEFDB5714}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C188BA3-B7F7-9A44-B21A-2B72A769B338}">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43BD365-7180-A842-86B4-2D807484C126}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>